<commit_message>
Diseño de Estructuras actualizado
</commit_message>
<xml_diff>
--- a/DisenoEstructurasCelayesVicentin.xlsx
+++ b/DisenoEstructurasCelayesVicentin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
   <si>
     <t>"palabraWordix"</t>
   </si>
@@ -101,9 +101,6 @@
     <t xml:space="preserve">$arregloResumen = </t>
   </si>
   <si>
-    <t>"partidas</t>
-  </si>
-  <si>
     <t>"puntajeTotal"</t>
   </si>
   <si>
@@ -186,13 +183,94 @@
   </si>
   <si>
     <t>¿Para qué se utiliza?: Es un arreglo para  almacenar palabras que van a ser utilizadas para jugar al WORDIX</t>
+  </si>
+  <si>
+    <t>INFORMACIÓN:</t>
+  </si>
+  <si>
+    <t>Integrantes:</t>
+  </si>
+  <si>
+    <t>Celayes, Brisa Abril</t>
+  </si>
+  <si>
+    <t>Vicentin, Juan</t>
+  </si>
+  <si>
+    <t>Legajos:</t>
+  </si>
+  <si>
+    <t>FAI-4923</t>
+  </si>
+  <si>
+    <t>FAI-5090</t>
+  </si>
+  <si>
+    <t>Mails:</t>
+  </si>
+  <si>
+    <t>brisacelayesabril@gmail.com</t>
+  </si>
+  <si>
+    <t>Nombre GITHUB:</t>
+  </si>
+  <si>
+    <t>abrilbc</t>
+  </si>
+  <si>
+    <t>juanfv5991</t>
+  </si>
+  <si>
+    <t>MUJER</t>
+  </si>
+  <si>
+    <t>FUEGO</t>
+  </si>
+  <si>
+    <t>RASGO</t>
+  </si>
+  <si>
+    <t>HUEVO</t>
+  </si>
+  <si>
+    <t>MELON</t>
+  </si>
+  <si>
+    <t>YUYOS</t>
+  </si>
+  <si>
+    <t>PIANO</t>
+  </si>
+  <si>
+    <t>PLATO</t>
+  </si>
+  <si>
+    <t>MILAN</t>
+  </si>
+  <si>
+    <t>DARIN</t>
+  </si>
+  <si>
+    <t>Tipo: Asociativo</t>
+  </si>
+  <si>
+    <t>Tipo de datos:</t>
+  </si>
+  <si>
+    <t>STRING ($nombre)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT ($partidasCont, $puntajeTotal, $victorias, $intento1, $intento2, $intento3, $intento4, $intento5, $intento6) </t>
+  </si>
+  <si>
+    <t>"partidas"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,8 +337,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,8 +390,18 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -306,14 +424,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -344,12 +509,26 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="8">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Encabezado 4" xfId="4" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="5" builtinId="20"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="6" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,484 +806,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.21875" customWidth="1"/>
     <col min="6" max="6" width="13.21875" customWidth="1"/>
     <col min="7" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>19</v>
-      </c>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B3" s="6">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="E8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B9" s="6">
         <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B6" s="6">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B7" s="6">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3">
-        <v>13</v>
-      </c>
-      <c r="F7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="6">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="6">
-        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3">
         <v>14</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B11" s="6">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B13" s="6">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3">
+        <v>13</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B14" s="6">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3">
+        <v>15</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B15" s="6">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3">
         <v>17</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F15" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="6">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B16" s="6">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E16" s="3">
         <v>17</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F16" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="6">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B17" s="6">
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E17" s="3">
         <v>17</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F17" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="6">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B18" s="6">
         <v>9</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E18" s="3">
         <v>11</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F18" s="3">
         <v>6</v>
       </c>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="J18" s="11"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4">
-        <f ca="1">C14:P150</f>
+      <c r="C21" s="4">
+        <f ca="1">C21:P150</f>
         <v>0</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D21" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E21" s="4">
         <v>2</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F21" s="4">
         <v>3</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G21" s="4">
         <v>4</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H21" s="4">
         <v>5</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I21" s="4">
         <v>6</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J21" s="4">
         <v>7</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K21" s="4">
         <v>8</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L21" s="4">
         <v>9</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M21" s="4">
         <v>10</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N21" s="4">
         <v>11</v>
       </c>
-      <c r="O14" s="4">
+      <c r="O21" s="4">
         <v>12</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P21" s="4">
         <v>13</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q21" s="4">
         <v>14</v>
       </c>
-      <c r="R14" s="4">
+      <c r="R21" s="4">
         <v>15</v>
       </c>
-      <c r="S14" s="4">
+      <c r="S21" s="4">
         <v>16</v>
       </c>
-      <c r="T14" s="4">
+      <c r="T21" s="4">
         <v>17</v>
       </c>
-      <c r="U14" s="4">
+      <c r="U21" s="4">
         <v>18</v>
       </c>
-      <c r="V14" s="4">
+      <c r="V21" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="V22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="V15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D30" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="G30" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="H30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="I30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="J30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="K30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="L30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="M30" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M24" s="8" t="s">
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
+      <c r="C31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="F31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="I31" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="J31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="K31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K25" s="9" t="s">
+      <c r="L31" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="L25" s="9" t="s">
+      <c r="M31" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="M25" s="9" t="s">
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>46</v>
       </c>
     </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>